<commit_message>
Lagergruppen mit erstem Test erstellt
</commit_message>
<xml_diff>
--- a/src/main/resources/base/owfw7/Test2_WarehouseGroupProperties.xlsx
+++ b/src/main/resources/base/owfw7/Test2_WarehouseGroupProperties.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>art</t>
   </si>
@@ -39,6 +39,9 @@
   </si>
   <si>
     <t>auftragsbezogen</t>
+  </si>
+  <si>
+    <t>umllg</t>
   </si>
 </sst>
 </file>
@@ -436,7 +439,7 @@
   <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -465,6 +468,9 @@
       <c r="C2" t="s">
         <v>3</v>
       </c>
+      <c r="D2" t="s">
+        <v>6</v>
+      </c>
       <c r="H2" s="1"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
@@ -477,6 +483,9 @@
       <c r="C3" t="s">
         <v>4</v>
       </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4">
@@ -487,6 +496,9 @@
       </c>
       <c r="C4" t="s">
         <v>5</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>